<commit_message>
Project ACC Master Offer is saved. Type: SAVE.
</commit_message>
<xml_diff>
--- a/DESIGN/rules/ACC Master Offer/rules/Offer Model.xlsx
+++ b/DESIGN/rules/ACC Master Offer/rules/Offer Model.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="10910"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kkalenik/Downloads/ACC Master Offer-Xia-2023-09-13_03-02-57 (1)/rules/"/>
     </mc:Choice>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1135" uniqueCount="917">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1150" uniqueCount="932">
   <si>
     <r>
       <rPr>
@@ -3438,11 +3438,57 @@
   <si>
     <t>String[] optionNames, ProductDimensions dimensions, Boolean scoped, CoveredOption[] inputAttributes</t>
   </si>
+  <si>
+    <t>MinMaxBehaviorInfo( behaviorDimensions = ProductBehaviorInfoDimensions( packages = behaviorPackages, plans = behaviorPlans, states = behaviorStates, coverages = behaviorCoverages, actions = behaviorActions), conditionName = behaviorConditionName, conditionValues = behaviorConditionValues, conditionExpression= $Expr.behaviorExpression.textValue, conditionExpressionResult = behaviorExpression, coveredOptionName = behaviorOptionName, minValue = minValue_, maxValue = maxValue_, incrementValue = incrementValue_, minExpression = "", maxExpression = "", incrementExpression = "" )</t>
+  </si>
+  <si>
+    <t>MinMaxBehaviorInfo( behaviorDimensions = ProductBehaviorInfoDimensions( packages = behaviorPackages, plans = behaviorPlans, states = behaviorStates, coverages = behaviorCoverages, actions = behaviorActions), conditionName = behaviorConditionName, conditionValues = behaviorConditionValues, conditionExpression= "", conditionExpressionResult = behaviorExpression, coveredOptionName = behaviorOptionName, minValue = minValue_, maxValue = maxValue_, incrementValue = incrementValue_, minExpression = "", maxExpression = "", incrementExpression = "" )</t>
+  </si>
+  <si>
+    <t>ApplicabilityBehaviorInfo( behaviorDimensions = ProductBehaviorInfoDimensions( actions = behaviorActions) , conditionName = behaviorConditionName, conditionValues = behaviorConditionValues, conditionExpression= "", conditionExpressionResult = behaviorExpression, entity = behaviorEntityName, discriminatorNames = discriminatorNames_, discriminatorValues = discriminatorValues_, applicabilityType = applicabilityType_, cardinality = cardinality_, ruleId = behaviorRuleId )</t>
+  </si>
+  <si>
+    <t>StringValuesBehaviorInfo( behaviorDimensions = ProductBehaviorInfoDimensions( packages = behaviorPackages, plans= behaviorPlans, states = behaviorStates, coverages = behaviorCoverages, actions = behaviorActions ) , conditionName = behaviorConditionName, conditionValues = behaviorConditionValues, conditionExpression= "", conditionExpressionResult = behaviorExpression,  coveredOptionName = behaviorOptionName, values = valuesRes_ , expression = "" )</t>
+  </si>
+  <si>
+    <t>StringValuesBehaviorInfo( behaviorDimensions = ProductBehaviorInfoDimensions( packages = behaviorPackages, plans= behaviorPlans, states = behaviorStates, coverages = behaviorCoverages, actions = behaviorActions ) , conditionName = behaviorConditionName, conditionValues = behaviorConditionValues, conditionExpression= "", conditionExpressionResult = behaviorExpression,  coveredOptionName = behaviorOptionName, values = values_ , expression = "")</t>
+  </si>
+  <si>
+    <t>MandatoryBehaviorInfo( behaviorDimensions = ProductBehaviorInfoDimensions( actions = behaviorActions), conditionName = behaviorConditionName, conditionValues = behaviorConditionValues, conditionExpression= "", conditionExpressionResult = behaviorExpression, coveredOptionName = behaviorOptionName, mandatory = mandatoryInd_, expression = "" )</t>
+  </si>
+  <si>
+    <t>MinMaxBehaviorInfo( behaviorDimensions = ProductBehaviorInfoDimensions( actions = behaviorActions) ,  conditionName = behaviorConditionName, conditionValues = behaviorConditionValues, conditionExpression= "", conditionExpressionResult = behaviorExpression, coveredOptionName = behaviorOptionName, minValue = minValueInd_, maxValue = maxValueInd_, incrementValue = incrementValueInd_, minExpression = "", maxExpression = $Expr.maxValueInd_.textValue, incrementExpression = "" )</t>
+  </si>
+  <si>
+    <t>MinMaxBehaviorInfo( behaviorDimensions = ProductBehaviorInfoDimensions( actions = behaviorActions) ,  conditionName = behaviorConditionName, conditionValues = behaviorConditionValues, conditionExpression= "", conditionExpressionResult = behaviorExpression, coveredOptionName = behaviorOptionName, minValue = minValueInd_, maxValue = maxValueInd_, incrementValue = incrementValueInd_, minExpression = "", maxExpression = "", incrementExpression = "" )</t>
+  </si>
+  <si>
+    <t>StringValuesBehaviorInfo( behaviorDimensions = ProductBehaviorInfoDimensions( actions = behaviorActions ) , conditionName = behaviorConditionName, conditionValues = behaviorConditionValues, conditionExpression= "", conditionExpressionResult = behaviorExpression,  coveredOptionName = behaviorOptionName, values = listValuesInd_ , expression = "" )</t>
+  </si>
+  <si>
+    <t>MandatoryBehaviorInfo( behaviorDimensions = ProductBehaviorInfoDimensions( packages = behaviorPackages, plans = behaviorPlans, states = behaviorStates, coverages = behaviorCoverages, actions = behaviorActions), conditionName = behaviorConditionName, conditionValues = behaviorConditionValues, conditionExpression= "", conditionExpressionResult = behaviorExpression, coveredOptionName = behaviorOptionName, mandatory = mandatory_, expression = "")</t>
+  </si>
+  <si>
+    <t>StringValuesBehaviorInfo( behaviorDimensions = ProductBehaviorInfoDimensions( actions = behaviorActions ) , conditionName = behaviorConditionName, conditionValues = behaviorConditionValues, conditionExpression= "", conditionExpressionResult = behaviorExpression,  coveredOptionName = behaviorOptionName, values = valuesResInd_ , expression = "" )</t>
+  </si>
+  <si>
+    <t>StringValuesBehaviorInfo( behaviorDimensions = ProductBehaviorInfoDimensions( packages = behaviorPackages, plans= behaviorPlans, states = behaviorStates, coverages = behaviorCoverages, actions = behaviorActions ) , conditionName = behaviorConditionName, conditionValues = behaviorConditionValues, conditionExpression= "", conditionExpressionResult = behaviorExpression,  coveredOptionName = behaviorOptionName, values = listValues_ , expression = "" )</t>
+  </si>
+  <si>
+    <t>StringValuesBehaviorInfo( behaviorDimensions = ProductBehaviorInfoDimensions( actions = behaviorActions ) , conditionName = behaviorConditionName, conditionValues = behaviorConditionValues, conditionExpression= $Expr.behaviorExpression.textValue, conditionExpressionResult = behaviorExpression,  coveredOptionName = behaviorOptionName, values = valuesInd_ , expression = "" )</t>
+  </si>
+  <si>
+    <t>StringValuesBehaviorInfo( behaviorDimensions = ProductBehaviorInfoDimensions( actions = behaviorActions ) , conditionName = behaviorConditionName, conditionValues = behaviorConditionValues, conditionExpression= "", conditionExpressionResult = behaviorExpression,  coveredOptionName = behaviorOptionName, values = valuesInd_ , expression = "" )</t>
+  </si>
+  <si>
+    <t>ApplicabilityBehaviorInfo( behaviorDimensions = ProductBehaviorInfoDimensions( packages = behaviorPackages, plans = behaviorPlans, states = behaviorStates, coverages = behaviorCoverages,  actions = behaviorActions ) , conditionName = behaviorConditionName, conditionValues = behaviorConditionValues, conditionExpression= "", conditionExpressionResult = behaviorExpression, entity = behaviorEntityName, discriminatorNames = discriminatorNames_, discriminatorValues = discriminatorValues_, applicabilityType = applicabilityType_, cardinality = cardinality_, ruleId = behaviorRuleId )</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="51">
     <font>
       <sz val="12"/>
@@ -3474,7 +3520,7 @@
     <font>
       <b/>
       <sz val="11"/>
-      <color theme="1"/>
+      <color theme="1" rgb="000000"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
     </font>
@@ -3486,7 +3532,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color theme="0" tint="-0.499984740745262"/>
+      <color theme="0" tint="-0.499984740745262" rgb="FFFFFF"/>
       <name val="Franklin Gothic Book"/>
       <family val="2"/>
     </font>
@@ -3879,7 +3925,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.39997558519241921"/>
+        <fgColor theme="8" tint="0.39997558519241921" rgb="5B9BD5"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -4162,26 +4208,26 @@
     </border>
     <border>
       <left style="thin">
-        <color theme="1"/>
+        <color theme="1" rgb="000000"/>
       </left>
       <right/>
       <top/>
       <bottom style="thin">
-        <color theme="1"/>
+        <color theme="1" rgb="000000"/>
       </bottom>
       <diagonal/>
     </border>
   </borders>
   <cellStyleXfs count="9">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="33" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="44" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="16" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0" xfId="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="17" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0" xfId="2"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="3"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="4"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0" xfId="5"/>
+    <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="6"/>
+    <xf numFmtId="0" fontId="44" fillId="0" borderId="0" xfId="7"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="8"/>
   </cellStyleXfs>
   <cellXfs count="138">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -4504,15 +4550,15 @@
     </xf>
   </cellXfs>
   <cellStyles count="9">
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Note 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
+    <cellStyle name="Normal 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="Normal 2" xfId="4" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
     <cellStyle name="Heading 1 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
-    <cellStyle name="Heading 2" xfId="2" builtinId="17"/>
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Normal 2" xfId="4" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
-    <cellStyle name="Normal 2 2" xfId="3" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
     <cellStyle name="Normal 2 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="Normal 3" xfId="7" xr:uid="{74AC3C1A-661C-F34D-B2CE-8CFFEBA168E2}"/>
     <cellStyle name="Normal 2 3" xfId="8" xr:uid="{12734518-A4A4-2D4F-8CF6-F930687B28FE}"/>
-    <cellStyle name="Normal 3" xfId="7" xr:uid="{74AC3C1A-661C-F34D-B2CE-8CFFEBA168E2}"/>
-    <cellStyle name="Note 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -4738,9 +4784,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="30.28515625" customWidth="1"/>
-    <col min="4" max="26" width="10.7109375" customWidth="1"/>
+    <col min="1" max="2" customWidth="true" width="10.7109375"/>
+    <col min="3" max="3" customWidth="true" width="30.28515625"/>
+    <col min="4" max="26" customWidth="true" width="10.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:3" ht="15" customHeight="1">
@@ -7891,10 +7937,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="1" width="3.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="4" width="25" customWidth="1"/>
-    <col min="5" max="26" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="3.7109375"/>
+    <col min="2" max="2" customWidth="true" width="10.7109375"/>
+    <col min="3" max="4" customWidth="true" width="25.0"/>
+    <col min="5" max="26" customWidth="true" width="10.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26">
@@ -27743,9 +27789,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="41.28515625" customWidth="1"/>
-    <col min="4" max="26" width="10.7109375" customWidth="1"/>
+    <col min="1" max="2" customWidth="true" width="10.7109375"/>
+    <col min="3" max="3" customWidth="true" width="41.28515625"/>
+    <col min="4" max="26" customWidth="true" width="10.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="15.75" customHeight="1">
@@ -55222,10 +55268,10 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="16"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" customWidth="1"/>
-    <col min="3" max="3" width="27.7109375" style="39" customWidth="1"/>
-    <col min="4" max="4" width="56.7109375" customWidth="1"/>
-    <col min="5" max="26" width="10.7109375" customWidth="1"/>
+    <col min="1" max="2" customWidth="true" width="10.7109375"/>
+    <col min="3" max="3" customWidth="true" style="39" width="27.7109375"/>
+    <col min="4" max="4" customWidth="true" width="56.7109375"/>
+    <col min="5" max="26" customWidth="true" width="10.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="3:7">
@@ -57991,12 +58037,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.28515625" defaultRowHeight="15" customHeight="1"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="28.85546875" customWidth="1"/>
-    <col min="3" max="3" width="27.42578125" customWidth="1"/>
-    <col min="4" max="4" width="10.7109375" customWidth="1"/>
-    <col min="5" max="5" width="27" customWidth="1"/>
-    <col min="6" max="26" width="10.7109375" customWidth="1"/>
+    <col min="1" max="1" customWidth="true" width="10.7109375"/>
+    <col min="2" max="2" customWidth="true" width="28.85546875"/>
+    <col min="3" max="3" customWidth="true" width="27.42578125"/>
+    <col min="4" max="4" customWidth="true" width="10.7109375"/>
+    <col min="5" max="5" customWidth="true" width="27.0"/>
+    <col min="6" max="26" customWidth="true" width="10.7109375"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:26" ht="16"/>
@@ -58620,12 +58666,12 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" style="1"/>
-    <col min="2" max="2" width="18.140625" style="1" customWidth="1"/>
-    <col min="3" max="3" width="42.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="21.140625" style="1" customWidth="1"/>
-    <col min="5" max="5" width="23.85546875" style="1" customWidth="1"/>
-    <col min="6" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="1" style="1" width="10.7109375"/>
+    <col min="2" max="2" customWidth="true" style="1" width="18.140625"/>
+    <col min="3" max="3" customWidth="true" style="1" width="42.85546875"/>
+    <col min="4" max="4" customWidth="true" style="1" width="21.140625"/>
+    <col min="5" max="5" customWidth="true" style="1" width="23.85546875"/>
+    <col min="6" max="16384" style="1" width="10.7109375"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:11" ht="20">
@@ -58929,7 +58975,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="16384" style="1" width="10.7109375"/>
   </cols>
   <sheetData>
     <row r="3" spans="2:2">
@@ -59034,9 +59080,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.42578125" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="2" width="9.42578125" style="74"/>
-    <col min="3" max="16" width="30" style="74" customWidth="1"/>
-    <col min="17" max="16384" width="9.42578125" style="74"/>
+    <col min="1" max="2" style="74" width="9.42578125"/>
+    <col min="3" max="16" customWidth="true" style="74" width="30.0"/>
+    <col min="17" max="16384" style="74" width="9.42578125"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:16">
@@ -59405,7 +59451,7 @@
         <v>786</v>
       </c>
       <c r="C38" s="127" t="s">
-        <v>846</v>
+        <v>931</v>
       </c>
       <c r="D38" s="128"/>
       <c r="E38" s="128"/>
@@ -59473,7 +59519,7 @@
         <v>786</v>
       </c>
       <c r="C46" s="123" t="s">
-        <v>856</v>
+        <v>919</v>
       </c>
       <c r="D46" s="124"/>
       <c r="E46" s="124"/>
@@ -59632,7 +59678,7 @@
         <v>786</v>
       </c>
       <c r="C67" s="89" t="s">
-        <v>913</v>
+        <v>921</v>
       </c>
     </row>
     <row r="68" spans="2:3" customFormat="1" ht="16">
@@ -59672,7 +59718,7 @@
         <v>786</v>
       </c>
       <c r="C74" s="89" t="s">
-        <v>874</v>
+        <v>930</v>
       </c>
     </row>
     <row r="75" spans="2:3" customFormat="1" ht="16">
@@ -59712,7 +59758,7 @@
         <v>786</v>
       </c>
       <c r="C81" s="89" t="s">
-        <v>878</v>
+        <v>928</v>
       </c>
     </row>
     <row r="82" spans="2:3" customFormat="1" ht="16">
@@ -59752,7 +59798,7 @@
         <v>786</v>
       </c>
       <c r="C88" s="89" t="s">
-        <v>881</v>
+        <v>925</v>
       </c>
     </row>
     <row r="89" spans="2:3" customFormat="1" ht="16">
@@ -59792,7 +59838,7 @@
         <v>786</v>
       </c>
       <c r="C95" s="89" t="s">
-        <v>885</v>
+        <v>920</v>
       </c>
     </row>
     <row r="96" spans="2:3" customFormat="1" ht="16">
@@ -59832,7 +59878,7 @@
         <v>786</v>
       </c>
       <c r="C102" s="89" t="s">
-        <v>889</v>
+        <v>927</v>
       </c>
     </row>
     <row r="103" spans="2:5" customFormat="1" ht="16">
@@ -59876,7 +59922,7 @@
         <v>786</v>
       </c>
       <c r="C109" s="115" t="s">
-        <v>893</v>
+        <v>918</v>
       </c>
       <c r="D109" s="116"/>
       <c r="E109" s="116"/>
@@ -59930,7 +59976,7 @@
         <v>786</v>
       </c>
       <c r="C116" s="111" t="s">
-        <v>899</v>
+        <v>924</v>
       </c>
       <c r="D116" s="112"/>
       <c r="E116" s="112"/>
@@ -59984,7 +60030,7 @@
         <v>786</v>
       </c>
       <c r="C123" s="89" t="s">
-        <v>915</v>
+        <v>926</v>
       </c>
     </row>
     <row r="124" spans="2:5" customFormat="1" ht="16">
@@ -60024,7 +60070,7 @@
         <v>786</v>
       </c>
       <c r="C130" s="89" t="s">
-        <v>910</v>
+        <v>922</v>
       </c>
     </row>
     <row r="131" spans="2:3" customFormat="1" ht="16">
@@ -60093,9 +60139,9 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.7109375" defaultRowHeight="14"/>
   <cols>
-    <col min="1" max="2" width="10.7109375" style="1"/>
-    <col min="3" max="3" width="17.140625" style="1" customWidth="1"/>
-    <col min="4" max="16384" width="10.7109375" style="1"/>
+    <col min="1" max="2" style="1" width="10.7109375"/>
+    <col min="3" max="3" customWidth="true" style="1" width="17.140625"/>
+    <col min="4" max="16384" style="1" width="10.7109375"/>
   </cols>
   <sheetData>
     <row r="4" spans="2:3">

</xml_diff>